<commit_message>
Replace Picture X with image and keep rest of question text
</commit_message>
<xml_diff>
--- a/questions1.xlsx
+++ b/questions1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roman\Программирование\test-with-password\alphatest2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B81F4D4-8983-44CE-A412-D6C31DB48102}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E62F123-0FD4-4EC9-A347-1C481E405CC9}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Questions" sheetId="1" r:id="rId1"/>
@@ -1106,8 +1106,8 @@
   </sheetPr>
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1814,7 +1814,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Split picture and question text in questions1.xlsx and questions2.xlsx
</commit_message>
<xml_diff>
--- a/questions1.xlsx
+++ b/questions1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roman\Программирование\test-with-password\alphatest2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E62F123-0FD4-4EC9-A347-1C481E405CC9}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9739C9ED-C828-4EE9-BDAA-54B58632F7B0}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="92">
   <si>
     <t>Топографічна карта це ...</t>
   </si>
@@ -265,148 +265,43 @@
     <t>input</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve">Picture 1. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>Який магнітний азимут встановлений на компасі?</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve">Picture 2. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>Визначте географічні координати вказаної точки. Широту та довготу вказувати градуси, хвилини та секунди через кому баз пробілів, наприклад, 52,37,40,31,37,20</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>Picture 3.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve"> Визначте повні прямокутні координати вказаної точки. Координати осі абсцис Х та координати осі ординат Y вказувати через пробіл. Приклад: 5455500 5612750</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>Picture 4.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve"> Чому буде дорівнювати азимут магнітний (Ам) якщо схилення на 2002 рік східне 10°15' (1-71), середнє відхилення меридіанів західне 2° 10' (0-36), а річна зміна схилення східна 0°04' (0-01)?</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>Picture 5.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve"> Визначте дирекційний кут направлення</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve">Picture 6. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>Переведіть дирекційний кут направлення в азимут магнітний. Запишіть значення в градусах та хвилинах через кому. Приклад: 132,24</t>
-    </r>
+    <t>Picture</t>
+  </si>
+  <si>
+    <t>Який магнітний азимут встановлений на компасі?</t>
+  </si>
+  <si>
+    <t>Picture 1</t>
+  </si>
+  <si>
+    <t>Picture 5</t>
+  </si>
+  <si>
+    <t>Визначте географічні координати вказаної точки. Широту та довготу вказувати градуси, хвилини та секунди через кому баз пробілів, наприклад, 52,37,40,31,37,20</t>
+  </si>
+  <si>
+    <t>Picture 2</t>
+  </si>
+  <si>
+    <t>Визначте повні прямокутні координати вказаної точки. Координати осі абсцис Х та координати осі ординат Y вказувати через пробіл. Приклад: 5455500 5612750</t>
+  </si>
+  <si>
+    <t>Picture 3</t>
+  </si>
+  <si>
+    <t>Picture 4</t>
+  </si>
+  <si>
+    <t>Чому буде дорівнювати азимут магнітний (Ам) якщо схилення на 2002 рік східне 10°15' (1-71), середнє відхилення меридіанів західне 2° 10' (0-36), а річна зміна схилення східна 0°04' (0-01)?</t>
+  </si>
+  <si>
+    <t>Визначте дирекційний кут направлення</t>
+  </si>
+  <si>
+    <t>Переведіть дирекційний кут направлення в азимут магнітний. Запишіть значення в градусах та хвилинах через кому. Приклад: 132,24</t>
+  </si>
+  <si>
+    <t>Picture 6</t>
   </si>
 </sst>
 </file>
@@ -444,8 +339,6 @@
       <charset val="204"/>
     </font>
     <font>
-      <b/>
-      <i/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -454,12 +347,14 @@
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="204"/>
+      <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -488,14 +383,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -504,8 +399,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1104,577 +1002,599 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.140625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="32.42578125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="30" style="5" customWidth="1"/>
-    <col min="4" max="4" width="35" style="5" customWidth="1"/>
-    <col min="5" max="5" width="31.85546875" style="5" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" style="5" customWidth="1"/>
-    <col min="8" max="9" width="41.42578125" style="5" customWidth="1"/>
-    <col min="10" max="10" width="33" style="5" customWidth="1"/>
-    <col min="11" max="11" width="22.85546875" style="5" customWidth="1"/>
-    <col min="12" max="16384" width="12.5703125" style="5"/>
+    <col min="1" max="1" width="12.5703125" style="5"/>
+    <col min="2" max="2" width="30.140625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="32.42578125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="30" style="5" customWidth="1"/>
+    <col min="5" max="5" width="35" style="5" customWidth="1"/>
+    <col min="6" max="6" width="31.85546875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" style="5" customWidth="1"/>
+    <col min="9" max="10" width="41.42578125" style="5" customWidth="1"/>
+    <col min="11" max="11" width="33" style="5" customWidth="1"/>
+    <col min="12" max="12" width="22.85546875" style="5" customWidth="1"/>
+    <col min="13" max="16384" width="12.5703125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:13" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="C2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="6"/>
       <c r="J2" s="6"/>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="6"/>
+      <c r="L2" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="L2" s="5">
+      <c r="M2" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:13" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="B3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="C3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="D3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="E3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="I3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="6"/>
       <c r="J3" s="6"/>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="6"/>
+      <c r="L3" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="L3" s="5">
+      <c r="M3" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="51" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="B4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="C4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="D4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="E4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="F4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="I4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="J4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="6"/>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="6"/>
+      <c r="L4" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="L4" s="5">
+      <c r="M4" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:13" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="C5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="D5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="E5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="F5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="I5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="6"/>
       <c r="J5" s="6"/>
-      <c r="K5" s="2" t="s">
+      <c r="K5" s="6"/>
+      <c r="L5" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="L5" s="5">
+      <c r="M5" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+    <row r="6" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="B6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="C6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="D6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="E6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="F6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="I6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="I6" s="6"/>
       <c r="J6" s="6"/>
-      <c r="K6" s="2" t="s">
+      <c r="K6" s="6"/>
+      <c r="L6" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="L6" s="5">
+      <c r="M6" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
+    <row r="7" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="B7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="C7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="D7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="E7" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="F7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="I7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I7" s="6"/>
       <c r="J7" s="6"/>
-      <c r="K7" s="2" t="s">
+      <c r="K7" s="6"/>
+      <c r="L7" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="L7" s="5">
+      <c r="M7" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:13" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B8" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="C8" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="D8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="E8" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="F8" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="I8" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="I8" s="6"/>
       <c r="J8" s="6"/>
-      <c r="K8" s="2" t="s">
+      <c r="K8" s="6"/>
+      <c r="L8" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="L8" s="5">
+      <c r="M8" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
+    <row r="9" spans="1:13" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B9" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="C9" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="D9" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="E9" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="F9" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="G9" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="H9" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="I9" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="I9" s="6" t="s">
+      <c r="J9" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="J9" s="6" t="s">
+      <c r="K9" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="L9" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="L9" s="5">
+      <c r="M9" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
+    <row r="10" spans="1:13" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B10" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="C10" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="D10" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="E10" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="F10" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="G10" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="H10" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="I10" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="I10" s="6"/>
       <c r="J10" s="6"/>
-      <c r="K10" s="2" t="s">
+      <c r="K10" s="6"/>
+      <c r="L10" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="L10" s="5">
+      <c r="M10" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
+    <row r="11" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B11" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="C11" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="D11" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="E11" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="F11" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="I11" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="I11" s="6"/>
       <c r="J11" s="6"/>
-      <c r="K11" s="2" t="s">
+      <c r="K11" s="6"/>
+      <c r="L11" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="L11" s="5">
+      <c r="M11" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
+    <row r="12" spans="1:13" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="B12" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="C12" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="D12" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="E12" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="F12" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="I12" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="I12" s="6"/>
       <c r="J12" s="6"/>
-      <c r="K12" s="2" t="s">
+      <c r="K12" s="6"/>
+      <c r="L12" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="L12" s="5">
+      <c r="M12" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
+    <row r="13" spans="1:13" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="B13" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="C13" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="D13" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="E13" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="F13" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="I13" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="I13" s="6"/>
       <c r="J13" s="6"/>
-      <c r="K13" s="2" t="s">
+      <c r="K13" s="6"/>
+      <c r="L13" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="L13" s="5">
+      <c r="M13" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
+    <row r="14" spans="1:13" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B14" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="C14" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="D14" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="E14" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="F14" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="H14" s="6" t="s">
+      <c r="I14" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="I14" s="6"/>
       <c r="J14" s="6"/>
-      <c r="K14" s="2" t="s">
+      <c r="K14" s="6"/>
+      <c r="L14" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="L14" s="5">
+      <c r="M14" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="51" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
+    <row r="15" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="B15" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="C15" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="D15" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="E15" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="F15" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="H15" s="6" t="s">
+      <c r="I15" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="I15" s="6"/>
       <c r="J15" s="6"/>
-      <c r="K15" s="2" t="s">
+      <c r="K15" s="6"/>
+      <c r="L15" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="L15" s="5">
+      <c r="M15" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A16" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="H16" s="6">
+    <row r="16" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I16" s="6">
         <v>154</v>
       </c>
-      <c r="I16" s="6"/>
       <c r="J16" s="6"/>
-      <c r="K16" s="2" t="s">
+      <c r="K16" s="6"/>
+      <c r="L16" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="L16" s="5">
+      <c r="M16" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A17" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="H17" s="6" t="s">
+    <row r="17" spans="1:13" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="I17" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="I17" s="6"/>
       <c r="J17" s="6"/>
-      <c r="K17" s="2" t="s">
+      <c r="K17" s="6"/>
+      <c r="L17" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="L17" s="5">
+      <c r="M17" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A18" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="H18" s="6" t="s">
+    <row r="18" spans="1:13" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="I18" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="I18" s="6"/>
       <c r="J18" s="6"/>
-      <c r="K18" s="2" t="s">
+      <c r="K18" s="6"/>
+      <c r="L18" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="L18" s="5">
+      <c r="M18" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A19" s="7" t="s">
+    <row r="19" spans="1:13" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="M19" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="L19" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A20" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="H20" s="6">
+      <c r="B20" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="I20" s="6">
         <v>240</v>
       </c>
-      <c r="I20" s="6"/>
       <c r="J20" s="6"/>
-      <c r="K20" s="2" t="s">
+      <c r="K20" s="6"/>
+      <c r="L20" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="L20" s="5">
+      <c r="M20" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A21" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="H21" s="6">
+    <row r="21" spans="1:13" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="I21" s="6">
         <v>229.43</v>
       </c>
-      <c r="I21" s="6"/>
       <c r="J21" s="6"/>
-      <c r="K21" s="2" t="s">
+      <c r="K21" s="6"/>
+      <c r="L21" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="L21" s="5">
+      <c r="M21" s="5">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update timer, add answer highlight, confirm modal, and progress line
</commit_message>
<xml_diff>
--- a/questions1.xlsx
+++ b/questions1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roman\Программирование\test-with-password\alphatest2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9739C9ED-C828-4EE9-BDAA-54B58632F7B0}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6176B7A2-A1F1-44FA-A1CC-8A366F9B8EB2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="110">
   <si>
     <t>Топографічна карта це ...</t>
   </si>
@@ -302,6 +302,60 @@
   </si>
   <si>
     <t>Picture 6</t>
+  </si>
+  <si>
+    <t>Option 7</t>
+  </si>
+  <si>
+    <t>Option 8</t>
+  </si>
+  <si>
+    <t>Option 9</t>
+  </si>
+  <si>
+    <t>Option 10</t>
+  </si>
+  <si>
+    <t>Option 11</t>
+  </si>
+  <si>
+    <t>Option 12</t>
+  </si>
+  <si>
+    <t>CorrectAnswer4</t>
+  </si>
+  <si>
+    <t>CorrectAnswer5</t>
+  </si>
+  <si>
+    <t>Як приготувати каву?</t>
+  </si>
+  <si>
+    <t>Налити води у чайник</t>
+  </si>
+  <si>
+    <t>Закипьятити чайник</t>
+  </si>
+  <si>
+    <t>Налити кипьяток у чашку</t>
+  </si>
+  <si>
+    <t>Добавити до кипьятка кави</t>
+  </si>
+  <si>
+    <t>Запарити каву</t>
+  </si>
+  <si>
+    <t>Покласти цукор</t>
+  </si>
+  <si>
+    <t>Перемышати цукор</t>
+  </si>
+  <si>
+    <t>Добавити кориці</t>
+  </si>
+  <si>
+    <t>ordering</t>
   </si>
 </sst>
 </file>
@@ -1002,10 +1056,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:U22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="M16" workbookViewId="0">
+      <selection activeCell="T25" sqref="T25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1017,14 +1071,14 @@
     <col min="5" max="5" width="35" style="5" customWidth="1"/>
     <col min="6" max="6" width="31.85546875" style="5" customWidth="1"/>
     <col min="7" max="7" width="19.42578125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" style="5" customWidth="1"/>
-    <col min="9" max="10" width="41.42578125" style="5" customWidth="1"/>
-    <col min="11" max="11" width="33" style="5" customWidth="1"/>
-    <col min="12" max="12" width="22.85546875" style="5" customWidth="1"/>
-    <col min="13" max="16384" width="12.5703125" style="5"/>
+    <col min="8" max="14" width="17.7109375" style="5" customWidth="1"/>
+    <col min="15" max="16" width="41.42578125" style="5" customWidth="1"/>
+    <col min="17" max="19" width="33" style="5" customWidth="1"/>
+    <col min="20" max="20" width="22.85546875" style="5" customWidth="1"/>
+    <col min="21" max="16384" width="12.5703125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>79</v>
       </c>
@@ -1049,23 +1103,47 @@
       <c r="H1" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="O1" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="R1" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="T1" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" ht="76.5" x14ac:dyDescent="0.2">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -1081,19 +1159,21 @@
       <c r="F2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="O2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="2" t="s">
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="M2" s="5">
+      <c r="U2" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="63.75" x14ac:dyDescent="0.2">
       <c r="B3" s="6" t="s">
         <v>5</v>
       </c>
@@ -1106,19 +1186,21 @@
       <c r="E3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="O3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="2" t="s">
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="M3" s="5">
+      <c r="U3" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" ht="51" x14ac:dyDescent="0.2">
       <c r="B4" s="6" t="s">
         <v>9</v>
       </c>
@@ -1134,21 +1216,23 @@
       <c r="F4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="O4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="P4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="6"/>
-      <c r="L4" s="2" t="s">
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="M4" s="5">
+      <c r="U4" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B5" s="6" t="s">
         <v>14</v>
       </c>
@@ -1164,19 +1248,21 @@
       <c r="F5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="O5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="2" t="s">
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="M5" s="5">
+      <c r="U5" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" ht="51" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
         <v>19</v>
       </c>
@@ -1192,19 +1278,21 @@
       <c r="F6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="O6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="2" t="s">
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
+      <c r="T6" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="M6" s="5">
+      <c r="U6" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" ht="51" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
         <v>24</v>
       </c>
@@ -1220,19 +1308,21 @@
       <c r="F7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="O7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="2" t="s">
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="M7" s="5">
+      <c r="U7" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
         <v>25</v>
       </c>
@@ -1248,19 +1338,21 @@
       <c r="F8" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="O8" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="2" t="s">
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="M8" s="5">
+      <c r="U8" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
         <v>30</v>
       </c>
@@ -1282,23 +1374,31 @@
       <c r="H9" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="I9" s="6" t="s">
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="J9" s="6" t="s">
+      <c r="P9" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="K9" s="6" t="s">
+      <c r="Q9" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="L9" s="2" t="s">
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="M9" s="5">
+      <c r="U9" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
         <v>37</v>
       </c>
@@ -1320,19 +1420,27 @@
       <c r="H10" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="I10" s="6" t="s">
-        <v>32</v>
-      </c>
+      <c r="I10" s="6"/>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
-      <c r="L10" s="2" t="s">
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="M10" s="5">
+      <c r="U10" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
         <v>38</v>
       </c>
@@ -1348,19 +1456,21 @@
       <c r="F11" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="O11" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="2" t="s">
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+      <c r="T11" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="M11" s="5">
+      <c r="U11" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" ht="76.5" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
         <v>43</v>
       </c>
@@ -1376,19 +1486,21 @@
       <c r="F12" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="I12" s="6" t="s">
+      <c r="O12" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="2" t="s">
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6"/>
+      <c r="T12" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="M12" s="5">
+      <c r="U12" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" ht="76.5" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
         <v>48</v>
       </c>
@@ -1404,19 +1516,21 @@
       <c r="F13" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="I13" s="6" t="s">
+      <c r="O13" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="2" t="s">
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6"/>
+      <c r="T13" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="M13" s="5">
+      <c r="U13" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B14" s="6" t="s">
         <v>49</v>
       </c>
@@ -1432,19 +1546,21 @@
       <c r="F14" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="I14" s="6" t="s">
+      <c r="O14" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="2" t="s">
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="6"/>
+      <c r="T14" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="M14" s="5">
+      <c r="U14" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" ht="51" x14ac:dyDescent="0.2">
       <c r="B15" s="6" t="s">
         <v>54</v>
       </c>
@@ -1460,76 +1576,84 @@
       <c r="F15" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="I15" s="6" t="s">
+      <c r="O15" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="2" t="s">
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
+      <c r="S15" s="6"/>
+      <c r="T15" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="M15" s="5">
+      <c r="U15" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>81</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="I16" s="6">
+      <c r="O16" s="6">
         <v>154</v>
       </c>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="2" t="s">
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="M16" s="5">
+      <c r="U16" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>84</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="I17" s="6" t="s">
+      <c r="O17" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="2" t="s">
+      <c r="P17" s="6"/>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="6"/>
+      <c r="S17" s="6"/>
+      <c r="T17" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="M17" s="5">
+      <c r="U17" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:21" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>86</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="I18" s="6" t="s">
+      <c r="O18" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="2" t="s">
+      <c r="P18" s="6"/>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="6"/>
+      <c r="S18" s="6"/>
+      <c r="T18" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="M18" s="5">
+      <c r="U18" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:21" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>87</v>
       </c>
@@ -1548,54 +1672,95 @@
       <c r="F19" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="I19" s="6" t="s">
+      <c r="O19" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="2" t="s">
+      <c r="P19" s="6"/>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="6"/>
+      <c r="S19" s="6"/>
+      <c r="T19" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="M19" s="5">
+      <c r="U19" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>82</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="I20" s="6">
+      <c r="O20" s="6">
         <v>240</v>
       </c>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="2" t="s">
+      <c r="P20" s="6"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6"/>
+      <c r="S20" s="6"/>
+      <c r="T20" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="M20" s="5">
+      <c r="U20" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:21" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>91</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="I21" s="6">
+      <c r="O21" s="6">
         <v>229.43</v>
       </c>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="2" t="s">
+      <c r="P21" s="6"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6"/>
+      <c r="S21" s="6"/>
+      <c r="T21" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="M21" s="5">
+      <c r="U21" s="5">
         <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="T22" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="U22" s="5">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update server.js, add questions files, and other changes
</commit_message>
<xml_diff>
--- a/questions1.xlsx
+++ b/questions1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roman\Программирование\test-with-password\alphatest2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B183EDE0-4A8D-4149-B3AA-E2CB85D4F34D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{973C03B0-A2A9-422B-B932-4CA8B38A0A06}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1052,8 +1052,8 @@
   </sheetPr>
   <dimension ref="A1:AB23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="AA22" sqref="AA22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1158,7 +1158,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="131.25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" ht="150" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1629,7 +1629,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="75" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" ht="93.75" x14ac:dyDescent="0.3">
       <c r="B14" s="4" t="s">
         <v>49</v>
       </c>
@@ -1731,7 +1731,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:28" ht="150" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:28" ht="168.75" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>81</v>
       </c>
@@ -1759,7 +1759,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:28" ht="150" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:28" ht="168.75" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>83</v>
       </c>
@@ -1787,7 +1787,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:28" ht="168.75" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:28" ht="187.5" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>84</v>
       </c>

</xml_diff>